<commit_message>
Made dashboard changes. Added presentation and building flask API
</commit_message>
<xml_diff>
--- a/Inputs/City_Geospatial_Data_Test.xlsx
+++ b/Inputs/City_Geospatial_Data_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bayer\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF5BC46-24E4-4055-AF43-0F5AC441EA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A78C263-5B5B-4942-97F7-DE0A0D57BAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{985C179B-B4DC-4D0D-BBEA-36EB6A3044FC}"/>
   </bookViews>
@@ -56,10 +56,10 @@
     <t>Elevation(In Feet)</t>
   </si>
   <si>
-    <t>Cambridge</t>
-  </si>
-  <si>
-    <t>Hebron</t>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Pittsburg</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,13 +492,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>42.485500000000002</v>
+        <v>33.3489</v>
       </c>
       <c r="C4">
-        <v>-71.391999999999996</v>
+        <v>-112.49120000000001</v>
       </c>
       <c r="D4" s="3">
-        <v>194</v>
+        <v>909</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,13 +506,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>42.324399999999997</v>
+        <v>40.468800000000002</v>
       </c>
       <c r="C5">
-        <v>-88.452399999999997</v>
+        <v>-79.981200000000001</v>
       </c>
       <c r="D5" s="3">
-        <v>1060</v>
+        <v>886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>